<commit_message>
commit 1.0 - preliminary dashboard complete
</commit_message>
<xml_diff>
--- a/data/protea_data.xlsx
+++ b/data/protea_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\campaign_dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A638622-68E9-4C49-AC2D-CC25363B5D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4575BE14-1F4C-445F-887D-A6A5D77D1526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FABB13C9-C832-45B1-A0E1-9426AF466A19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{FABB13C9-C832-45B1-A0E1-9426AF466A19}"/>
   </bookViews>
   <sheets>
     <sheet name="combat_per_session" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="132">
   <si>
     <t>combatant</t>
   </si>
@@ -434,9 +434,6 @@
   </si>
   <si>
     <t>NPC</t>
-  </si>
-  <si>
-    <t>spells_cast</t>
   </si>
 </sst>
 </file>
@@ -807,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33409C88-ED7A-494F-8A57-A214E4BDAB40}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
@@ -817,6 +814,8 @@
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5702,11 +5701,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876CBE52-1DED-432E-B73D-B8426A240A27}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5715,11 +5714,11 @@
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="105" customWidth="1"/>
+    <col min="8" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="105" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -5751,13 +5750,10 @@
         <v>126</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14</v>
       </c>
@@ -5788,11 +5784,11 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14</v>
       </c>
@@ -5823,11 +5819,11 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14</v>
       </c>
@@ -5858,11 +5854,11 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -5893,11 +5889,11 @@
       <c r="J5">
         <v>3</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
@@ -5928,7 +5924,7 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>